<commit_message>
fix a google translate data
</commit_message>
<xml_diff>
--- a/report/journal_result_2018_2.xlsx
+++ b/report/journal_result_2018_2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\journal_scraping\report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{370ACE91-ABC5-40A1-B041-41B89A8AD2E1}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BA37B66-248A-4716-804D-59D2C6D2401D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7935" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1464,15 +1464,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J105"/>
+  <dimension ref="A1:I105"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1497,11 +1497,11 @@
       <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -1526,11 +1526,11 @@
       <c r="H2" t="s">
         <v>183</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -1555,11 +1555,11 @@
       <c r="H3" t="s">
         <v>184</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -1584,11 +1584,11 @@
       <c r="H4" t="s">
         <v>185</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="I4" s="2" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -1613,11 +1613,11 @@
       <c r="H5" t="s">
         <v>186</v>
       </c>
-      <c r="J5" s="2" t="s">
+      <c r="I5" s="2" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -1642,11 +1642,11 @@
       <c r="H6" t="s">
         <v>187</v>
       </c>
-      <c r="J6" s="2" t="s">
+      <c r="I6" s="2" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -1671,11 +1671,11 @@
       <c r="H7" t="s">
         <v>188</v>
       </c>
-      <c r="J7" s="2" t="s">
+      <c r="I7" s="2" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -1700,11 +1700,11 @@
       <c r="H8" t="s">
         <v>189</v>
       </c>
-      <c r="J8" s="2" t="s">
+      <c r="I8" s="2" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -1729,11 +1729,11 @@
       <c r="H9" t="s">
         <v>190</v>
       </c>
-      <c r="J9" s="2" t="s">
+      <c r="I9" s="2" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -1758,11 +1758,11 @@
       <c r="H10" t="s">
         <v>191</v>
       </c>
-      <c r="J10" s="2" t="s">
+      <c r="I10" s="2" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -1787,11 +1787,11 @@
       <c r="H11" t="s">
         <v>192</v>
       </c>
-      <c r="J11" s="2" t="s">
+      <c r="I11" s="2" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -1816,11 +1816,11 @@
       <c r="H12" t="s">
         <v>193</v>
       </c>
-      <c r="J12" s="2" t="s">
+      <c r="I12" s="2" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -1845,11 +1845,11 @@
       <c r="H13" t="s">
         <v>194</v>
       </c>
-      <c r="J13" s="2" t="s">
+      <c r="I13" s="2" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>8</v>
       </c>
@@ -1874,11 +1874,11 @@
       <c r="H14" t="s">
         <v>195</v>
       </c>
-      <c r="J14" s="2" t="s">
+      <c r="I14" s="2" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>8</v>
       </c>
@@ -1903,11 +1903,11 @@
       <c r="H15" t="s">
         <v>196</v>
       </c>
-      <c r="J15" s="2" t="s">
+      <c r="I15" s="2" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>8</v>
       </c>
@@ -1932,11 +1932,11 @@
       <c r="H16" t="s">
         <v>197</v>
       </c>
-      <c r="J16" s="2" t="s">
+      <c r="I16" s="2" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>8</v>
       </c>
@@ -1961,11 +1961,11 @@
       <c r="H17" t="s">
         <v>198</v>
       </c>
-      <c r="J17" s="2" t="s">
+      <c r="I17" s="2" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>9</v>
       </c>
@@ -1990,11 +1990,11 @@
       <c r="H18" t="s">
         <v>199</v>
       </c>
-      <c r="J18" s="2" t="s">
+      <c r="I18" s="2" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>9</v>
       </c>
@@ -2019,11 +2019,11 @@
       <c r="H19" t="s">
         <v>200</v>
       </c>
-      <c r="J19" s="2" t="s">
+      <c r="I19" s="2" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>9</v>
       </c>
@@ -2048,11 +2048,11 @@
       <c r="H20" t="s">
         <v>201</v>
       </c>
-      <c r="J20" s="2" t="s">
+      <c r="I20" s="2" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>9</v>
       </c>
@@ -2077,11 +2077,11 @@
       <c r="H21" t="s">
         <v>202</v>
       </c>
-      <c r="J21" s="2" t="s">
+      <c r="I21" s="2" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>9</v>
       </c>
@@ -2106,11 +2106,11 @@
       <c r="H22" t="s">
         <v>203</v>
       </c>
-      <c r="J22" s="2" t="s">
+      <c r="I22" s="2" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>9</v>
       </c>
@@ -2135,11 +2135,11 @@
       <c r="H23" t="s">
         <v>204</v>
       </c>
-      <c r="J23" s="2" t="s">
+      <c r="I23" s="2" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>9</v>
       </c>
@@ -2164,11 +2164,11 @@
       <c r="H24" t="s">
         <v>205</v>
       </c>
-      <c r="J24" s="2" t="s">
+      <c r="I24" s="2" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>9</v>
       </c>
@@ -2193,11 +2193,11 @@
       <c r="H25" t="s">
         <v>206</v>
       </c>
-      <c r="J25" s="2" t="s">
+      <c r="I25" s="2" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>9</v>
       </c>
@@ -2222,11 +2222,11 @@
       <c r="H26" t="s">
         <v>207</v>
       </c>
-      <c r="J26" s="2" t="s">
+      <c r="I26" s="2" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>9</v>
       </c>
@@ -2251,11 +2251,11 @@
       <c r="H27" t="s">
         <v>208</v>
       </c>
-      <c r="J27" s="2" t="s">
+      <c r="I27" s="2" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>9</v>
       </c>
@@ -2280,11 +2280,11 @@
       <c r="H28" t="s">
         <v>209</v>
       </c>
-      <c r="J28" s="2" t="s">
+      <c r="I28" s="2" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>9</v>
       </c>
@@ -2309,11 +2309,11 @@
       <c r="H29" t="s">
         <v>210</v>
       </c>
-      <c r="J29" s="2" t="s">
+      <c r="I29" s="2" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>9</v>
       </c>
@@ -2338,11 +2338,11 @@
       <c r="H30" t="s">
         <v>211</v>
       </c>
-      <c r="J30" s="2" t="s">
+      <c r="I30" s="2" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>9</v>
       </c>
@@ -2367,11 +2367,11 @@
       <c r="H31" t="s">
         <v>212</v>
       </c>
-      <c r="J31" s="2" t="s">
+      <c r="I31" s="2" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>9</v>
       </c>
@@ -2396,11 +2396,11 @@
       <c r="H32" t="s">
         <v>213</v>
       </c>
-      <c r="J32" s="2" t="s">
+      <c r="I32" s="2" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>9</v>
       </c>
@@ -2425,11 +2425,11 @@
       <c r="H33" t="s">
         <v>214</v>
       </c>
-      <c r="J33" s="2" t="s">
+      <c r="I33" s="2" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>10</v>
       </c>
@@ -2454,11 +2454,11 @@
       <c r="H34" t="s">
         <v>215</v>
       </c>
-      <c r="J34" s="2" t="s">
+      <c r="I34" s="2" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>10</v>
       </c>
@@ -2483,11 +2483,11 @@
       <c r="H35" t="s">
         <v>216</v>
       </c>
-      <c r="J35" s="2" t="s">
+      <c r="I35" s="2" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>10</v>
       </c>
@@ -2512,11 +2512,11 @@
       <c r="H36" t="s">
         <v>217</v>
       </c>
-      <c r="J36" s="2" t="s">
+      <c r="I36" s="2" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>10</v>
       </c>
@@ -2541,11 +2541,11 @@
       <c r="H37" t="s">
         <v>218</v>
       </c>
-      <c r="J37" s="2" t="s">
+      <c r="I37" s="2" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>10</v>
       </c>
@@ -2570,11 +2570,11 @@
       <c r="H38" t="s">
         <v>219</v>
       </c>
-      <c r="J38" s="2" t="s">
+      <c r="I38" s="2" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>10</v>
       </c>
@@ -2599,11 +2599,11 @@
       <c r="H39" t="s">
         <v>220</v>
       </c>
-      <c r="J39" s="2" t="s">
+      <c r="I39" s="2" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>10</v>
       </c>
@@ -2628,11 +2628,11 @@
       <c r="H40" t="s">
         <v>221</v>
       </c>
-      <c r="J40" s="2" t="s">
+      <c r="I40" s="2" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>10</v>
       </c>
@@ -2657,11 +2657,11 @@
       <c r="H41" t="s">
         <v>222</v>
       </c>
-      <c r="J41" s="2" t="s">
+      <c r="I41" s="2" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="42" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>10</v>
       </c>
@@ -2686,11 +2686,11 @@
       <c r="H42" t="s">
         <v>223</v>
       </c>
-      <c r="J42" s="2" t="s">
+      <c r="I42" s="2" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>10</v>
       </c>
@@ -2715,11 +2715,11 @@
       <c r="H43" t="s">
         <v>224</v>
       </c>
-      <c r="J43" s="2" t="s">
+      <c r="I43" s="2" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="44" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>10</v>
       </c>
@@ -2744,11 +2744,11 @@
       <c r="H44" t="s">
         <v>225</v>
       </c>
-      <c r="J44" s="2" t="s">
+      <c r="I44" s="2" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="45" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>11</v>
       </c>
@@ -2773,11 +2773,11 @@
       <c r="H45" t="s">
         <v>226</v>
       </c>
-      <c r="J45" s="2" t="s">
+      <c r="I45" s="2" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="46" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>11</v>
       </c>
@@ -2802,11 +2802,11 @@
       <c r="H46" t="s">
         <v>227</v>
       </c>
-      <c r="J46" s="2" t="s">
+      <c r="I46" s="2" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="47" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>11</v>
       </c>
@@ -2831,11 +2831,11 @@
       <c r="H47" t="s">
         <v>228</v>
       </c>
-      <c r="J47" s="2" t="s">
+      <c r="I47" s="2" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="48" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>11</v>
       </c>
@@ -2860,11 +2860,11 @@
       <c r="H48" t="s">
         <v>229</v>
       </c>
-      <c r="J48" s="2" t="s">
+      <c r="I48" s="2" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="49" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>11</v>
       </c>
@@ -2889,11 +2889,11 @@
       <c r="H49" t="s">
         <v>230</v>
       </c>
-      <c r="J49" s="2" t="s">
+      <c r="I49" s="2" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="50" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>12</v>
       </c>
@@ -2918,11 +2918,11 @@
       <c r="H50" t="s">
         <v>231</v>
       </c>
-      <c r="J50" s="2" t="s">
+      <c r="I50" s="2" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="51" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>12</v>
       </c>
@@ -2947,11 +2947,11 @@
       <c r="H51" t="s">
         <v>232</v>
       </c>
-      <c r="J51" s="2" t="s">
+      <c r="I51" s="2" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="52" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>12</v>
       </c>
@@ -2976,11 +2976,11 @@
       <c r="H52" t="s">
         <v>233</v>
       </c>
-      <c r="J52" s="2" t="s">
+      <c r="I52" s="2" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="53" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>12</v>
       </c>
@@ -3005,11 +3005,11 @@
       <c r="H53" t="s">
         <v>234</v>
       </c>
-      <c r="J53" s="2" t="s">
+      <c r="I53" s="2" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="54" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>12</v>
       </c>
@@ -3034,11 +3034,11 @@
       <c r="H54" t="s">
         <v>235</v>
       </c>
-      <c r="J54" s="2" t="s">
+      <c r="I54" s="2" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="55" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>12</v>
       </c>
@@ -3063,11 +3063,11 @@
       <c r="H55" t="s">
         <v>236</v>
       </c>
-      <c r="J55" s="2" t="s">
+      <c r="I55" s="2" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="56" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>12</v>
       </c>
@@ -3092,11 +3092,11 @@
       <c r="H56" t="s">
         <v>237</v>
       </c>
-      <c r="J56" s="2" t="s">
+      <c r="I56" s="2" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="57" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>13</v>
       </c>
@@ -3121,11 +3121,11 @@
       <c r="H57" t="s">
         <v>238</v>
       </c>
-      <c r="J57" s="2" t="s">
+      <c r="I57" s="2" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="58" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>13</v>
       </c>
@@ -3150,11 +3150,11 @@
       <c r="H58" t="s">
         <v>239</v>
       </c>
-      <c r="J58" s="2" t="s">
+      <c r="I58" s="2" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="59" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>13</v>
       </c>
@@ -3179,11 +3179,11 @@
       <c r="H59" t="s">
         <v>240</v>
       </c>
-      <c r="J59" s="2" t="s">
+      <c r="I59" s="2" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="60" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>13</v>
       </c>
@@ -3208,11 +3208,11 @@
       <c r="H60" t="s">
         <v>241</v>
       </c>
-      <c r="J60" s="2" t="s">
+      <c r="I60" s="2" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="61" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>13</v>
       </c>
@@ -3237,11 +3237,11 @@
       <c r="H61" t="s">
         <v>242</v>
       </c>
-      <c r="J61" s="2" t="s">
+      <c r="I61" s="2" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="62" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>13</v>
       </c>
@@ -3266,11 +3266,11 @@
       <c r="H62" t="s">
         <v>243</v>
       </c>
-      <c r="J62" s="2" t="s">
+      <c r="I62" s="2" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="63" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>13</v>
       </c>
@@ -3295,11 +3295,11 @@
       <c r="H63" t="s">
         <v>244</v>
       </c>
-      <c r="J63" s="2" t="s">
+      <c r="I63" s="2" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="64" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>13</v>
       </c>
@@ -3324,11 +3324,11 @@
       <c r="H64" t="s">
         <v>245</v>
       </c>
-      <c r="J64" s="2" t="s">
+      <c r="I64" s="2" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="65" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>13</v>
       </c>
@@ -3353,11 +3353,11 @@
       <c r="H65" t="s">
         <v>246</v>
       </c>
-      <c r="J65" s="2" t="s">
+      <c r="I65" s="2" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="66" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>14</v>
       </c>
@@ -3382,11 +3382,11 @@
       <c r="H66" t="s">
         <v>247</v>
       </c>
-      <c r="J66" s="2" t="s">
+      <c r="I66" s="2" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="67" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>14</v>
       </c>
@@ -3411,11 +3411,11 @@
       <c r="H67" t="s">
         <v>248</v>
       </c>
-      <c r="J67" s="2" t="s">
+      <c r="I67" s="2" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="68" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>14</v>
       </c>
@@ -3440,11 +3440,11 @@
       <c r="H68" t="s">
         <v>249</v>
       </c>
-      <c r="J68" s="2" t="s">
+      <c r="I68" s="2" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="69" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>14</v>
       </c>
@@ -3469,11 +3469,11 @@
       <c r="H69" t="s">
         <v>250</v>
       </c>
-      <c r="J69" s="2" t="s">
+      <c r="I69" s="2" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="70" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>14</v>
       </c>
@@ -3498,11 +3498,11 @@
       <c r="H70" t="s">
         <v>251</v>
       </c>
-      <c r="J70" s="2" t="s">
+      <c r="I70" s="2" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="71" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>14</v>
       </c>
@@ -3527,11 +3527,11 @@
       <c r="H71" t="s">
         <v>252</v>
       </c>
-      <c r="J71" s="2" t="s">
+      <c r="I71" s="2" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="72" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>14</v>
       </c>
@@ -3556,11 +3556,11 @@
       <c r="H72" t="s">
         <v>253</v>
       </c>
-      <c r="J72" s="2" t="s">
+      <c r="I72" s="2" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="73" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>14</v>
       </c>
@@ -3585,11 +3585,11 @@
       <c r="H73" t="s">
         <v>254</v>
       </c>
-      <c r="J73" s="2" t="s">
+      <c r="I73" s="2" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="74" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>14</v>
       </c>
@@ -3614,11 +3614,11 @@
       <c r="H74" t="s">
         <v>255</v>
       </c>
-      <c r="J74" s="2" t="s">
+      <c r="I74" s="2" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="75" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>14</v>
       </c>
@@ -3643,11 +3643,11 @@
       <c r="H75" t="s">
         <v>256</v>
       </c>
-      <c r="J75" s="2" t="s">
+      <c r="I75" s="2" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="76" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>14</v>
       </c>
@@ -3672,11 +3672,11 @@
       <c r="H76" t="s">
         <v>257</v>
       </c>
-      <c r="J76" s="2" t="s">
+      <c r="I76" s="2" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="77" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>14</v>
       </c>
@@ -3701,11 +3701,11 @@
       <c r="H77" t="s">
         <v>257</v>
       </c>
-      <c r="J77" s="2" t="s">
+      <c r="I77" s="2" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="78" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>14</v>
       </c>
@@ -3730,11 +3730,11 @@
       <c r="H78" t="s">
         <v>258</v>
       </c>
-      <c r="J78" s="2" t="s">
+      <c r="I78" s="2" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="79" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>14</v>
       </c>
@@ -3759,11 +3759,11 @@
       <c r="H79" t="s">
         <v>259</v>
       </c>
-      <c r="J79" s="2" t="s">
+      <c r="I79" s="2" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="80" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>14</v>
       </c>
@@ -3788,11 +3788,11 @@
       <c r="H80" t="s">
         <v>260</v>
       </c>
-      <c r="J80" s="2" t="s">
+      <c r="I80" s="2" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="81" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>14</v>
       </c>
@@ -3817,11 +3817,11 @@
       <c r="H81" t="s">
         <v>261</v>
       </c>
-      <c r="J81" s="2" t="s">
+      <c r="I81" s="2" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="82" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>14</v>
       </c>
@@ -3846,11 +3846,11 @@
       <c r="H82" t="s">
         <v>262</v>
       </c>
-      <c r="J82" s="2" t="s">
+      <c r="I82" s="2" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="83" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>14</v>
       </c>
@@ -3875,11 +3875,11 @@
       <c r="H83" t="s">
         <v>263</v>
       </c>
-      <c r="J83" s="2" t="s">
+      <c r="I83" s="2" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="84" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>14</v>
       </c>
@@ -3904,72 +3904,72 @@
       <c r="H84" t="s">
         <v>264</v>
       </c>
-      <c r="J84" s="2" t="s">
+      <c r="I84" s="2" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="85" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J85" s="3"/>
-    </row>
-    <row r="86" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J86" s="3"/>
-    </row>
-    <row r="87" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J87" s="3"/>
-    </row>
-    <row r="88" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J88" s="3"/>
-    </row>
-    <row r="89" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J89" s="3"/>
-    </row>
-    <row r="90" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J90" s="3"/>
-    </row>
-    <row r="91" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J91" s="3"/>
-    </row>
-    <row r="92" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J92" s="3"/>
-    </row>
-    <row r="93" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J93" s="3"/>
-    </row>
-    <row r="94" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J94" s="3"/>
-    </row>
-    <row r="95" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J95" s="3"/>
-    </row>
-    <row r="96" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J96" s="3"/>
-    </row>
-    <row r="97" spans="10:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J97" s="3"/>
-    </row>
-    <row r="98" spans="10:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J98" s="3"/>
-    </row>
-    <row r="99" spans="10:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J99" s="3"/>
-    </row>
-    <row r="100" spans="10:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J100" s="3"/>
-    </row>
-    <row r="101" spans="10:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J101" s="3"/>
-    </row>
-    <row r="102" spans="10:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J102" s="3"/>
-    </row>
-    <row r="103" spans="10:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J103" s="3"/>
-    </row>
-    <row r="104" spans="10:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J104" s="3"/>
-    </row>
-    <row r="105" spans="10:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J105" s="3"/>
+    <row r="85" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I85" s="3"/>
+    </row>
+    <row r="86" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I86" s="3"/>
+    </row>
+    <row r="87" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I87" s="3"/>
+    </row>
+    <row r="88" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I88" s="3"/>
+    </row>
+    <row r="89" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I89" s="3"/>
+    </row>
+    <row r="90" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I90" s="3"/>
+    </row>
+    <row r="91" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I91" s="3"/>
+    </row>
+    <row r="92" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I92" s="3"/>
+    </row>
+    <row r="93" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I93" s="3"/>
+    </row>
+    <row r="94" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I94" s="3"/>
+    </row>
+    <row r="95" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I95" s="3"/>
+    </row>
+    <row r="96" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I96" s="3"/>
+    </row>
+    <row r="97" spans="9:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I97" s="3"/>
+    </row>
+    <row r="98" spans="9:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I98" s="3"/>
+    </row>
+    <row r="99" spans="9:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I99" s="3"/>
+    </row>
+    <row r="100" spans="9:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I100" s="3"/>
+    </row>
+    <row r="101" spans="9:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I101" s="3"/>
+    </row>
+    <row r="102" spans="9:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I102" s="3"/>
+    </row>
+    <row r="103" spans="9:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I103" s="3"/>
+    </row>
+    <row r="104" spans="9:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I104" s="3"/>
+    </row>
+    <row r="105" spans="9:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I105" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>